<commit_message>
Tomcat installation on App server is completed
</commit_message>
<xml_diff>
--- a/Notes/Issues/Multi Tier Web Application Setup - Debug.xlsx
+++ b/Notes/Issues/Multi Tier Web Application Setup - Debug.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Tool</t>
   </si>
@@ -47,6 +47,47 @@
   </si>
   <si>
     <t>.\Notes\Issues\Vagrant.1</t>
+  </si>
+  <si>
+    <t>Tomcat</t>
+  </si>
+  <si>
+    <t>tomcat.service lacks both ExecStart= and ExecStop= setting. Refusing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(code=exited, status=203/EXEC) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit the tomcat.service and write the below lines:
+ExecStart=/usr/local/tomcat/bin/catalina.sh run
+ExecStop=/usr/local/tomcat/bin/shutdown.sh
+SyslogIdentifier=tomcat-%i
+</t>
+  </si>
+  <si>
+    <t>.\Notes\Issues\Tomcat.1</t>
+  </si>
+  <si>
+    <t>.\Notes\Issues\Tomcat.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tomcat.service file didn’t had the below lines  :
+ExecStart=/usr/local/tomcat/bin/catalina.sh run
+ExecStop=/usr/local/tomcat/bin/shutdown.sh
+SyslogIdentifier=tomcat-%i
+</t>
+  </si>
+  <si>
+    <t>tomcat.service file had wrong path for ExecStart &amp; ExecStop :
+ExecStart=/usr/local/tomcat/bin/catalina.sh run
+ExecStop=/usr/local/tomcat/bin/shutdown.sh
+SyslogIdentifier=tomcat-%i</t>
+  </si>
+  <si>
+    <t>Edit the tomcat.service and write the below lines:
+ExecStart=/usr/local/tomcat/bin/catalina.sh run
+ExecStop=/usr/local/tomcat/bin/shutdown.sh
+SyslogIdentifier=tomcat-%i</t>
   </si>
 </sst>
 </file>
@@ -111,9 +152,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -419,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,6 +516,40 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>